<commit_message>
Little change in WorkHours file
</commit_message>
<xml_diff>
--- a/WorkHours.xlsx
+++ b/WorkHours.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giulio\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renzu\Desktop\SoftEng2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,12 +29,6 @@
     <t xml:space="preserve">Melloni Giulio </t>
   </si>
   <si>
-    <t>Marco Renzi</t>
-  </si>
-  <si>
-    <t>Filippo Testa</t>
-  </si>
-  <si>
     <t>FROM</t>
   </si>
   <si>
@@ -45,6 +39,12 @@
   </si>
   <si>
     <t>HOURS</t>
+  </si>
+  <si>
+    <t>Renzi Marco</t>
+  </si>
+  <si>
+    <t>Testa Filippo</t>
   </si>
 </sst>
 </file>
@@ -109,13 +109,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -435,7 +435,7 @@
   <dimension ref="B2:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="32" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -444,39 +444,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4"/>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="2:7" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>42669</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>0.5</v>
       </c>
       <c r="E4" s="1">

</xml_diff>